<commit_message>
modify by zcn 2020-01-01
</commit_message>
<xml_diff>
--- a/craw_datas/Craw_souhu文献属性.xlsx
+++ b/craw_datas/Craw_souhu文献属性.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>标志</t>
   </si>
@@ -49,103 +49,100 @@
     <t>后缀</t>
   </si>
   <si>
-    <t>CRA20191216212144</t>
-  </si>
-  <si>
-    <t>CRA201912162121440001</t>
-  </si>
-  <si>
-    <t>CRA201912162121440002</t>
-  </si>
-  <si>
-    <t>CRA201912162121440003</t>
-  </si>
-  <si>
-    <t>CRA201912162121440004</t>
-  </si>
-  <si>
-    <t>CRA201912162121440005</t>
-  </si>
-  <si>
-    <t>CRA201912162121440006</t>
-  </si>
-  <si>
-    <t>CRA201912162121440007</t>
-  </si>
-  <si>
-    <t>CRA201912162121440008</t>
-  </si>
-  <si>
-    <t>CRA201912162121440009</t>
-  </si>
-  <si>
-    <t>CRA201912162121440010</t>
-  </si>
-  <si>
-    <t>大量建造052D的背后：海军规模虽大，但舰艇没有一艘能达到先进水平</t>
-  </si>
-  <si>
-    <t>美国对中国渐露狰狞！85次演习绕家门口转 助纣为虐者必遭重击</t>
-  </si>
-  <si>
-    <t>向太空发射5亿根铜针，距今已有60年，“西福特”计划现状如何？</t>
-  </si>
-  <si>
-    <t>美国突然插手，亚洲强国暴乱失控！军警街头开火射死多人</t>
-  </si>
-  <si>
-    <t>两中国外交官因“间谍活动”被美驱逐？耿爽：对我人员指责严重违背事实，强烈敦促美方撤销有关决定</t>
-  </si>
-  <si>
-    <t>美国人评出全球五大海军排名，中国名次引人关注，获得高度评价</t>
-  </si>
-  <si>
-    <t>印度骚乱持续升级！阿萨姆邦已有6人死亡，有4人死在警察枪口下</t>
-  </si>
-  <si>
-    <t>骚乱升级，印度警方攻入国立伊斯兰大学</t>
-  </si>
-  <si>
-    <t>翼龙无人机再次出击 导弹击中土耳其一弹药库 大批武器弹药被炸毁</t>
-  </si>
-  <si>
-    <t>当战局不利之际 俄叙联军投掷300多枚大炸弹 叛军被炸得支离破碎</t>
-  </si>
-  <si>
-    <t>2019-12-15</t>
-  </si>
-  <si>
-    <t>2019-12-16</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360277111_120126853</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360729884_366952</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360557412_120126853</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360747964_120312037</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360722399_162522</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360745380_762801</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360738389_100143040</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360758443_115479</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360493651_120163841</t>
-  </si>
-  <si>
-    <t>http://www.sohu.com/a/360633028_120163841</t>
+    <t>CRA20191227194043</t>
+  </si>
+  <si>
+    <t>CRA201912271940430001</t>
+  </si>
+  <si>
+    <t>CRA201912271940430002</t>
+  </si>
+  <si>
+    <t>CRA201912271940430003</t>
+  </si>
+  <si>
+    <t>CRA201912271940430004</t>
+  </si>
+  <si>
+    <t>CRA201912271940430005</t>
+  </si>
+  <si>
+    <t>CRA201912271940430006</t>
+  </si>
+  <si>
+    <t>CRA201912271940430007</t>
+  </si>
+  <si>
+    <t>CRA201912271940430008</t>
+  </si>
+  <si>
+    <t>CRA201912271940430009</t>
+  </si>
+  <si>
+    <t>CRA201912271940430010</t>
+  </si>
+  <si>
+    <t>以色列这次真捅了马蜂窝，179枚导弹连番轰炸，这才是真正苦战</t>
+  </si>
+  <si>
+    <t>卫星曝印度边境突现神秘基地：印军紧急侦察，却发现屏幕一片模糊</t>
+  </si>
+  <si>
+    <t>乌克兰又在大甩卖？价格十分尴尬，大国不需要，小国买不起</t>
+  </si>
+  <si>
+    <t>联合国大会上，中方一票否决西方提案，美当初阻扰马达西奇终于遭报复</t>
+  </si>
+  <si>
+    <t>后悔拒绝中方索赔，波音CEO被炒鱿鱼，留下最后2句忠告</t>
+  </si>
+  <si>
+    <t>投票再次通过，特朗普正式签名，大局已定，白宫终于松一口气</t>
+  </si>
+  <si>
+    <t>美国确认制裁俄欧天然气管道，个别欧企立刻停工，俄提前留了一手</t>
+  </si>
+  <si>
+    <t>韩国制造不靠谱！挪威27500吨巨舰曝重大缺陷，服役不久就被禁航</t>
+  </si>
+  <si>
+    <t>印巴突然交火，中方有何评论？外交部回应</t>
+  </si>
+  <si>
+    <t>20万吨！今年中国海军下水吨位又是世界第一</t>
+  </si>
+  <si>
+    <t>2019-12-27</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363188949_120147869</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363175748_100145375</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363150133_120157852</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363162539_637401</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363189846_120098002</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363138524_100018095</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363182702_100143135</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363174104_120113110</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363148524_162522</t>
+  </si>
+  <si>
+    <t>http://www.sohu.com/a/363182424_115479</t>
   </si>
 </sst>
 </file>
@@ -571,7 +568,7 @@
         <v>32</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -585,10 +582,10 @@
         <v>23</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -602,10 +599,10 @@
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -619,10 +616,10 @@
         <v>25</v>
       </c>
       <c r="I5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -636,10 +633,10 @@
         <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -653,10 +650,10 @@
         <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -670,10 +667,10 @@
         <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -687,10 +684,10 @@
         <v>29</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -704,10 +701,10 @@
         <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -721,10 +718,10 @@
         <v>31</v>
       </c>
       <c r="I11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>